<commit_message>
first model attempt departures
</commit_message>
<xml_diff>
--- a/region_mapping.xlsx
+++ b/region_mapping.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joe\Documents\Data Analytics Bootcamp\99_Final_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joe\Documents\Data Analytics Bootcamp\99_Final_Project\final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DCBC5F-565D-43C1-92CC-4735C10BF7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC11373-4B1E-4AE1-8C8B-DF07B61654B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{935AD596-7D71-4A43-B25A-EA5FA6480618}"/>
   </bookViews>
@@ -466,7 +466,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>